<commit_message>
WIP let us try potential
</commit_message>
<xml_diff>
--- a/src/lithium/data/ValeursFinalesCinetiqueMolarite.xlsx
+++ b/src/lithium/data/ValeursFinalesCinetiqueMolarite.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13840" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37500" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cinétique" sheetId="1" r:id="rId1"/>
+    <sheet name="Dose réponse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>MOYENNES Neptune + et AA</t>
   </si>
@@ -36,10 +37,54 @@
     <t>AA</t>
   </si>
   <si>
-    <t>mM Intracellulaire</t>
+    <t>ratio pentes NHE1-PS120</t>
   </si>
   <si>
-    <t>ratio pentes NHE1-PS120</t>
+    <t>mM NHE1</t>
+  </si>
+  <si>
+    <t>mM PS120</t>
+  </si>
+  <si>
+    <t>Delta 7</t>
+  </si>
+  <si>
+    <t>Ecartype</t>
+  </si>
+  <si>
+    <t>MOYENNES NEPTUNE+</t>
+  </si>
+  <si>
+    <t>Li Externe</t>
+  </si>
+  <si>
+    <t>mM Li Intracellulaire</t>
+  </si>
+  <si>
+    <t>Moyennes Delta 7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SEM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -50,13 +95,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,6 +129,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
     </font>
   </fonts>
   <fills count="5">
@@ -128,40 +171,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="37">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -173,6 +232,13 @@
     <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -184,6 +250,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -205,22 +278,22 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$4</c:f>
+              <c:f>Cinétique!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mM Intracellulaire</c:v>
+                  <c:v>mM NHE1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -241,7 +314,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$B$5:$B$10</c:f>
+              <c:f>Cinétique!$B$5:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -268,7 +341,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$5:$C$10</c:f>
+              <c:f>Cinétique!$C$5:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -289,6 +362,79 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>48.2487951858154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Cinétique!$I$5:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Cinétique!$J$5:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.549727827416667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.660515206592956</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.38405927787476</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.63525359670671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.40439583697911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -303,11 +449,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2047621624"/>
-        <c:axId val="-2068349272"/>
+        <c:axId val="-2143341544"/>
+        <c:axId val="-2144777112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2047621624"/>
+        <c:axId val="-2143341544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,11 +470,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Time</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="fr-FR" baseline="0"/>
-                  <a:t> (s)</a:t>
+                  <a:t>Time (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -340,12 +482,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2068349272"/>
+        <c:crossAx val="-2144777112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2068349272"/>
+        <c:axId val="-2144777112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -362,13 +504,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Intracellular Li</a:t>
+                  <a:t>Intracellular Li (mM)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="fr-FR" baseline="0"/>
-                  <a:t> (mM)</a:t>
-                </a:r>
-                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -379,7 +516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2047621624"/>
+        <c:crossAx val="-2143341544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -410,66 +547,216 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Cinétique!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mM NHE1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$E$5:$E$10</c:f>
+              <c:f>Cinétique!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>30.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>180.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>360.0</c:v>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3600.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$F$5:$F$10</c:f>
+              <c:f>Cinétique!$C$5:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5.111751074033566</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.49354190056044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.68418710400193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.2174044765961</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.2487951858154</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76.98146118562051</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>101.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.51925079240514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Cinétique!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mM PS120</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Cinétique!$I$5:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2400.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2700.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3600.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Cinétique!$J$5:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.549727827416667</c:v>
                 </c:pt>
                 <c:pt idx="2">
@@ -483,6 +770,27 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.40439583697911</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.28472840111605</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.918150250986</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.9269941132672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.1526879444444</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.7433352175765</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.7848311388889</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.2369372751923</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,13 +805,452 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2068273784"/>
-        <c:axId val="-2068209464"/>
+        <c:axId val="2062847000"/>
+        <c:axId val="2062854680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2068273784"/>
+        <c:axId val="2062847000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400" baseline="0"/>
+                  <a:t> (s) </a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062854680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2062854680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400" b="1" i="0" baseline="0"/>
+                  <a:t>Intracellular Li mM</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1400" b="1" i="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062847000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.782129165672473"/>
+          <c:y val="0.423937007874016"/>
+          <c:w val="0.0908867073434002"/>
+          <c:h val="0.101557084125546"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Cinétique!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delta 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Cinétique!$B$4:$B$14</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Temps</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3600</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Cinétique!$D$4:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="2">
+                  <c:v>1.002612155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83019506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.700639666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5671284</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.67866165</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5365548</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.640273</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.244714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2146460728"/>
+        <c:axId val="-2146457688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2146460728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2146457688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2146457688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2146460728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dose réponse'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mM Li Intracellulaire</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dose réponse'!$B$4:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dose réponse'!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.139622922372436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.148493240542579</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.30335663702284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.09869680600734</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.2246653980667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.28193386248208</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68.1892670972604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2144152104"/>
+        <c:axId val="-2144157832"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2144152104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -518,8 +1265,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Time (s)</a:t>
+                  <a:t>Extracellular</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> Li+ (mM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -530,12 +1282,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2068209464"/>
+        <c:crossAx val="-2144157832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2068209464"/>
+        <c:axId val="-2144157832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,8 +1304,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Intracellular Li (mM)</a:t>
+                  <a:t>Intracellula</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t>r Li+ (mM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -564,15 +1321,258 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2068273784"/>
+        <c:crossAx val="-2144152104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dose réponse'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Moyennes Delta 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dose réponse'!$B$4:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dose réponse'!$D$4:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="1">
+                  <c:v>4.89100787271542</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.88254556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.978844572681671</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.32449782</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.42556975</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.43460705</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.092503615</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6108183</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2144187976"/>
+        <c:axId val="-2144193704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2144187976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200"/>
+                  <a:t>Extracellular Li+</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1200" baseline="0"/>
+                  <a:t> (mM)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2144193704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2144193704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400">
+                    <a:latin typeface="Symbol" charset="2"/>
+                    <a:cs typeface="Symbol" charset="2"/>
+                  </a:rPr>
+                  <a:t>d</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400"/>
+                  <a:t>7 Li</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.116666666666667"/>
+              <c:y val="0.077438393117527"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2144187976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -585,16 +1585,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -615,20 +1615,115 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Graphique 9"/>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -971,56 +2066,72 @@
   <dimension ref="B1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F17"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:10">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="5">
-        <f>0.7822/0.0175</f>
-        <v>44.69714285714285</v>
+      <c r="J4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -1030,10 +2141,14 @@
       <c r="C5" s="2">
         <v>0.04</v>
       </c>
-      <c r="E5" s="1">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="1">
+      <c r="J5" s="1">
         <v>0.04</v>
       </c>
     </row>
@@ -1044,10 +2159,18 @@
       <c r="C6" s="2">
         <v>5.1117510740335668</v>
       </c>
-      <c r="E6" s="1">
+      <c r="D6" s="2">
+        <v>1.002612155</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.44235857061803352</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="1">
         <v>15</v>
       </c>
-      <c r="F6" s="1">
+      <c r="J6" s="1">
         <v>0.54972782741666704</v>
       </c>
     </row>
@@ -1058,10 +2181,18 @@
       <c r="C7" s="2">
         <v>10.493541900560444</v>
       </c>
-      <c r="E7" s="1">
+      <c r="D7" s="2">
+        <v>0.83019505999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.29737848030130076</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="1">
         <v>30</v>
       </c>
-      <c r="F7" s="1">
+      <c r="J7" s="1">
         <v>0.66051520659295604</v>
       </c>
     </row>
@@ -1072,10 +2203,18 @@
       <c r="C8" s="2">
         <v>14.68418710400193</v>
       </c>
-      <c r="E8" s="1">
+      <c r="D8" s="2">
+        <v>1.7006396666666668</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.71522609551590199</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="1">
         <v>60</v>
       </c>
-      <c r="F8" s="1">
+      <c r="J8" s="1">
         <v>1.38405927787476</v>
       </c>
     </row>
@@ -1086,10 +2225,18 @@
       <c r="C9" s="2">
         <v>24.217404476596091</v>
       </c>
-      <c r="E9" s="1">
+      <c r="D9" s="2">
+        <v>1.5671283999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.19295704367262798</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="1">
         <v>180</v>
       </c>
-      <c r="F9" s="1">
+      <c r="J9" s="1">
         <v>3.6352535967067099</v>
       </c>
     </row>
@@ -1100,10 +2247,18 @@
       <c r="C10" s="2">
         <v>48.248795185815396</v>
       </c>
-      <c r="E10" s="1">
+      <c r="D10" s="2">
+        <v>2.67866165</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.19941280970801492</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="1">
         <v>360</v>
       </c>
-      <c r="F10" s="1">
+      <c r="J10" s="1">
         <v>6.4043958369791101</v>
       </c>
     </row>
@@ -1114,10 +2269,14 @@
       <c r="C11" s="2">
         <v>76.981461185620518</v>
       </c>
-      <c r="E11" s="1">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="I11" s="1">
         <v>600</v>
       </c>
-      <c r="F11" s="1">
+      <c r="J11" s="1">
         <v>9.28472840111605</v>
       </c>
     </row>
@@ -1128,24 +2287,36 @@
       <c r="C12" s="2">
         <v>101</v>
       </c>
-      <c r="E12" s="1">
+      <c r="D12" s="2">
+        <v>7.5365548000000002</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="1">
         <v>1200</v>
       </c>
-      <c r="F12" s="1">
+      <c r="J12" s="1">
         <v>13.918150250986001</v>
       </c>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>1500</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="7">
         <v>108</v>
       </c>
-      <c r="E13" s="1">
+      <c r="D13" s="2">
+        <v>12.640273000000001</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="I13" s="1">
         <v>1800</v>
       </c>
-      <c r="F13" s="1">
+      <c r="J13" s="1">
         <v>15.926994113267201</v>
       </c>
     </row>
@@ -1156,34 +2327,49 @@
       <c r="C14" s="2">
         <v>88.519250792405145</v>
       </c>
-      <c r="E14" s="1">
+      <c r="D14" s="2">
+        <v>13.244714</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.7344056804862524</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="I14" s="1">
         <v>2400</v>
       </c>
-      <c r="F14" s="1">
+      <c r="J14" s="1">
         <v>18.152687944444398</v>
       </c>
     </row>
     <row r="15" spans="2:10">
-      <c r="E15" s="1">
+      <c r="I15" s="1">
         <v>2700</v>
       </c>
-      <c r="F15" s="1">
+      <c r="J15" s="1">
         <v>18.743335217576501</v>
       </c>
     </row>
     <row r="16" spans="2:10">
-      <c r="E16" s="1">
+      <c r="F16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <f>0.7822/0.0175</f>
+        <v>44.69714285714285</v>
+      </c>
+      <c r="I16" s="1">
         <v>3000</v>
       </c>
-      <c r="F16" s="1">
+      <c r="J16" s="1">
         <v>20.784831138888901</v>
       </c>
     </row>
-    <row r="17" spans="5:6">
-      <c r="E17" s="1">
+    <row r="17" spans="9:10">
+      <c r="I17" s="1">
         <v>3600</v>
       </c>
-      <c r="F17" s="1">
+      <c r="J17" s="1">
         <v>22.2369372751923</v>
       </c>
     </row>
@@ -1197,4 +2383,162 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="16">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.1396229223724357</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5">
+        <v>0.3</v>
+      </c>
+      <c r="C5">
+        <v>5.148493240542579</v>
+      </c>
+      <c r="D5">
+        <v>4.89100787271542</v>
+      </c>
+      <c r="E5">
+        <v>0.67486020496625188</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>10.303356637022842</v>
+      </c>
+      <c r="D6">
+        <v>3.8825455599999996</v>
+      </c>
+      <c r="E6">
+        <v>0.68452573764027214</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>21.098696806007339</v>
+      </c>
+      <c r="D7">
+        <v>3.9788445726816715</v>
+      </c>
+      <c r="E7">
+        <v>0.59759974627725942</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>48.25</v>
+      </c>
+      <c r="D8">
+        <v>3.3244978199999999</v>
+      </c>
+      <c r="E8">
+        <v>0.84214608662409773</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>62.224665398066705</v>
+      </c>
+      <c r="D9">
+        <v>1.4255697500000002</v>
+      </c>
+      <c r="E9">
+        <v>0.33209195583013407</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>64.281933862482077</v>
+      </c>
+      <c r="D10">
+        <v>1.4346070499999999</v>
+      </c>
+      <c r="E10">
+        <v>0.12322916287441549</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>68.189267097260398</v>
+      </c>
+      <c r="D11">
+        <v>1.092503615</v>
+      </c>
+      <c r="E11">
+        <v>0.11719696198154674</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12">
+        <v>120</v>
+      </c>
+      <c r="D12">
+        <v>1.6108183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>